<commit_message>
Added v1.2 of valve block
</commit_message>
<xml_diff>
--- a/03_Pneumatics/HollandValve/opening calculation.xlsx
+++ b/03_Pneumatics/HollandValve/opening calculation.xlsx
@@ -16,26 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>depth neg</t>
   </si>
   <si>
-    <t>pressure controlled valve a</t>
-  </si>
-  <si>
-    <t>pressure controlled valve b</t>
-  </si>
-  <si>
-    <t>pressure controlled valve c</t>
-  </si>
-  <si>
-    <t>one way valve b</t>
-  </si>
-  <si>
-    <t>one way valve c</t>
-  </si>
-  <si>
     <t>top corridor</t>
   </si>
   <si>
@@ -57,10 +42,43 @@
     <t>2 x 13 holes</t>
   </si>
   <si>
-    <t>area inside hosetail 19 mm</t>
-  </si>
-  <si>
-    <t>area inside hosetail 12.7 mm</t>
+    <t>number of channels in bottom</t>
+  </si>
+  <si>
+    <t>individual channel width in bottom</t>
+  </si>
+  <si>
+    <t>area inside hosetail 16 mm</t>
+  </si>
+  <si>
+    <t>pressure controlled valve type a</t>
+  </si>
+  <si>
+    <t>pressure controlled valve type b</t>
+  </si>
+  <si>
+    <t>pressure controlled valve type c</t>
+  </si>
+  <si>
+    <t>one way valve type b</t>
+  </si>
+  <si>
+    <t>one way valve type c</t>
+  </si>
+  <si>
+    <t>area inside hosetail 19.5 mm</t>
+  </si>
+  <si>
+    <t>area inside hosetail 13.5 mm</t>
+  </si>
+  <si>
+    <t>mini one way valve</t>
+  </si>
+  <si>
+    <t>&lt;-</t>
+  </si>
+  <si>
+    <t>oval via</t>
   </si>
 </sst>
 </file>
@@ -393,19 +411,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C13"/>
+  <dimension ref="A3:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -413,100 +432,149 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
         <f>PI()/4*(16.5*16.5)</f>
         <v>213.8246499849553</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <f>PI()/4*(10.2*10.2)</f>
-        <v>81.712824919870513</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>PI()/4*(13*13)</f>
+        <v>132.73228961416876</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <f>PI()/4*(10.5*10.5)</f>
+        <v>86.59014751456867</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
         <f>PI()/4*12*12+12*12</f>
         <v>257.09733552923257</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
         <f>13*(PI()/4*3*3)</f>
         <v>91.89158511750145</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <f>0.6*B7</f>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>0.6*B10</f>
         <v>154.25840131753952</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
         <f>15*(PI()/4*3*3)</f>
         <v>106.02875205865551</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <f>6*PI()/4*(5.5*5.5) + PI()/4*(4*4)</f>
-        <v>155.11613727099603</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <f>0.5*(16.5*8.25)+(16.5*6.25)</f>
-        <v>171.1875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <f>3*(6*(B3-1-3)+0.5*6*3)</f>
-        <v>171</v>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <f>6*PI()/4*(5*5) + PI()/4*(4.5*4.5)</f>
+        <v>133.71403731841556</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <f>PI()/4*10*10+10*7</f>
+        <v>148.53981633974485</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <f>2*(PI()/4*4.5*4.5)</f>
+        <v>31.808625617596654</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <f>0.5*(17*(15-6.5))+(17*6.5)</f>
+        <v>182.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f>$B$4*($B$5*($B$3-$B$5/2)+0.125*$B$5*$B$5)-2*0.5*0.5*0.5</f>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>